<commit_message>
Update based on FWSpecies output
-Add genus field to FWSpecies report and update scripts accordingly
-Move Ctenicera kendalli to FWSpecies
-Fill in missing scientific name values
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="18195" windowHeight="4125" tabRatio="358" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="108" windowWidth="18198" windowHeight="4128" tabRatio="358" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rules of Behavior" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="147">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -518,6 +518,21 @@
   </si>
   <si>
     <t>https://www.gbif.org/species/4469083</t>
+  </si>
+  <si>
+    <t>Pseudanostirus ochreipennis (LeConte, 1863)</t>
+  </si>
+  <si>
+    <t>Pseudanostirus ochreipennis</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Pseudanostirus&lt;/em&gt; &lt;em&gt;ochreipennis&lt;/em&gt; (LeConte, 1863)</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Pseudanostirus&lt;/em&gt; &lt;em&gt;ochreipennis&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/6981137</t>
   </si>
 </sst>
 </file>
@@ -1160,97 +1175,97 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="169.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="169.578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
         <v>47</v>
       </c>
@@ -1265,32 +1280,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="86.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.41796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.26171875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.41796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.15625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.15625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.26171875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.41796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="86.578125" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="47" style="12" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="4"/>
+    <col min="14" max="16384" width="8.83984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
@@ -1331,7 +1346,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1360,7 +1375,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1389,7 +1404,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1418,7 +1433,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1447,7 +1462,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1474,6 +1489,35 @@
       </c>
       <c r="M6" s="12" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1006311</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1538,25 +1582,25 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="86.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="9"/>
+    <col min="2" max="2" width="21.578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.41796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.26171875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.41796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.15625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.15625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.26171875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.41796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="86.578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.68359375" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="8.83984375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
@@ -1597,7 +1641,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7">
         <v>43758</v>
       </c>
@@ -1632,7 +1676,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -1659,7 +1703,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1694,7 +1738,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7">
         <v>22</v>
       </c>
@@ -1727,7 +1771,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8">
         <v>23</v>
       </c>
@@ -1760,7 +1804,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8">
         <v>24</v>
       </c>
@@ -1795,7 +1839,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8">
         <v>25</v>
       </c>
@@ -1894,16 +1938,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -1920,7 +1964,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1938,7 +1982,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1956,7 +2000,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1974,7 +2018,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1992,7 +2036,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Genus</v>
@@ -2007,7 +2051,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Subgenus</v>
@@ -2022,7 +2066,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Species</v>
@@ -2037,7 +2081,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Subspecies</v>
@@ -2052,7 +2096,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Variety</v>
@@ -2067,7 +2111,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Form</v>
@@ -2082,7 +2126,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Race</v>
@@ -2097,7 +2141,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Stirp</v>
@@ -2112,7 +2156,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Morph</v>
@@ -2127,7 +2171,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Aberration</v>
@@ -2142,7 +2186,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Unspecified</v>
@@ -2157,7 +2201,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Family</v>
@@ -2172,7 +2216,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subfamily</v>
@@ -2187,7 +2231,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Tribe</v>
@@ -2202,7 +2246,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subtribe</v>
@@ -2217,7 +2261,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Genus</v>
@@ -2232,7 +2276,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subgenus</v>
@@ -2247,7 +2291,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Species</v>
@@ -2262,7 +2306,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subspecies</v>
@@ -2277,7 +2321,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Family</v>
@@ -2292,7 +2336,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subfamily</v>
@@ -2307,7 +2351,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Tribe</v>
@@ -2322,7 +2366,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subtribe</v>
@@ -2337,7 +2381,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Genus</v>
@@ -2352,7 +2396,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subgenus</v>
@@ -2367,7 +2411,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Species</v>
@@ -2382,7 +2426,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subspecies</v>
@@ -2397,7 +2441,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Unspecified</v>
@@ -2412,7 +2456,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Family</v>
@@ -2427,7 +2471,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subfamily</v>
@@ -2442,7 +2486,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C36" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Tribe</v>
@@ -2457,7 +2501,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C37" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subtribe</v>
@@ -2472,7 +2516,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Genus</v>
@@ -2487,7 +2531,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subgenus</v>
@@ -2502,7 +2546,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C40" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Species</v>
@@ -2517,7 +2561,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C41" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subspecies</v>
@@ -2532,7 +2576,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Variety</v>
@@ -2547,7 +2591,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Form</v>
@@ -2562,7 +2606,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C44" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Race</v>
@@ -2577,7 +2621,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Stirp</v>
@@ -2592,7 +2636,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Morph</v>
@@ -2607,7 +2651,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C47" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Aberration</v>
@@ -2622,7 +2666,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Unspecified</v>
@@ -2637,7 +2681,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Family</v>
@@ -2652,7 +2696,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C50" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subfamily</v>
@@ -2667,7 +2711,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C51" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Tribe</v>
@@ -2682,7 +2726,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C52" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subtribe</v>
@@ -2697,7 +2741,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C53" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Genus</v>
@@ -2712,7 +2756,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C54" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subgenus</v>
@@ -2727,7 +2771,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C55" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Section</v>
@@ -2742,7 +2786,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C56" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subsection</v>
@@ -2757,7 +2801,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C57" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Species</v>
@@ -2772,7 +2816,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C58" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subspecies</v>
@@ -2787,7 +2831,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C59" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Variety</v>
@@ -2802,7 +2846,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C60" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subvariety</v>
@@ -2817,7 +2861,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C61" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Form</v>
@@ -2832,7 +2876,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C62" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subform</v>
@@ -2847,7 +2891,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C63" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Unspecified</v>
@@ -2862,7 +2906,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" t="str">
         <f t="shared" si="0"/>
         <v>Crab/Lobster/Shrimp|Family</v>
@@ -2877,7 +2921,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C65" t="str">
         <f t="shared" si="0"/>
         <v>Crab/Lobster/Shrimp|Subfamily</v>
@@ -2892,7 +2936,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C66" t="str">
         <f t="shared" ref="C66:C129" si="1">D66&amp;"|"&amp;E66</f>
         <v>Crab/Lobster/Shrimp|Tribe</v>
@@ -2907,7 +2951,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subtribe</v>
@@ -2922,7 +2966,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Genus</v>
@@ -2937,7 +2981,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subgenus</v>
@@ -2952,7 +2996,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Species</v>
@@ -2967,7 +3011,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C71" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subspecies</v>
@@ -2982,7 +3026,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C72" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Variety</v>
@@ -2997,7 +3041,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C73" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Form</v>
@@ -3012,7 +3056,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C74" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Race</v>
@@ -3027,7 +3071,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C75" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Stirp</v>
@@ -3042,7 +3086,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C76" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Morph</v>
@@ -3057,7 +3101,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C77" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Aberration</v>
@@ -3072,7 +3116,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C78" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Unspecified</v>
@@ -3087,7 +3131,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C79" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Family</v>
@@ -3102,7 +3146,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C80" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subfamily</v>
@@ -3117,7 +3161,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C81" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Tribe</v>
@@ -3132,7 +3176,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C82" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subtribe</v>
@@ -3147,7 +3191,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C83" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Genus</v>
@@ -3162,7 +3206,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C84" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subgenus</v>
@@ -3177,7 +3221,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C85" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Species</v>
@@ -3192,7 +3236,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C86" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subspecies</v>
@@ -3207,7 +3251,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C87" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Variety</v>
@@ -3222,7 +3266,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C88" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Form</v>
@@ -3237,7 +3281,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C89" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Race</v>
@@ -3252,7 +3296,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C90" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Stirp</v>
@@ -3267,7 +3311,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C91" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Morph</v>
@@ -3282,7 +3326,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C92" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Aberration</v>
@@ -3297,7 +3341,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C93" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Unspecified</v>
@@ -3312,7 +3356,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C94" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Family</v>
@@ -3327,7 +3371,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C95" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subfamily</v>
@@ -3342,7 +3386,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C96" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Tribe</v>
@@ -3357,7 +3401,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C97" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subtribe</v>
@@ -3372,7 +3416,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C98" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Genus</v>
@@ -3387,7 +3431,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C99" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subgenus</v>
@@ -3402,7 +3446,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C100" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Section</v>
@@ -3417,7 +3461,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C101" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subsection</v>
@@ -3432,7 +3476,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C102" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Species</v>
@@ -3447,7 +3491,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C103" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subspecies</v>
@@ -3462,7 +3506,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C104" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Variety</v>
@@ -3477,7 +3521,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C105" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subvariety</v>
@@ -3492,7 +3536,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C106" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Form</v>
@@ -3507,7 +3551,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C107" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subform</v>
@@ -3522,7 +3566,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C108" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Unspecified</v>
@@ -3537,7 +3581,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C109" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Family</v>
@@ -3552,7 +3596,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C110" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subfamily</v>
@@ -3567,7 +3611,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C111" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Tribe</v>
@@ -3582,7 +3626,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C112" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subtribe</v>
@@ -3597,7 +3641,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C113" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Genus</v>
@@ -3612,7 +3656,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C114" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subgenus</v>
@@ -3627,7 +3671,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C115" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Species</v>
@@ -3642,7 +3686,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C116" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subspecies</v>
@@ -3657,7 +3701,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C117" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Variety</v>
@@ -3672,7 +3716,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C118" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Form</v>
@@ -3687,7 +3731,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C119" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Race</v>
@@ -3702,7 +3746,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C120" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Stirp</v>
@@ -3717,7 +3761,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C121" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Morph</v>
@@ -3732,7 +3776,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C122" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Aberration</v>
@@ -3747,7 +3791,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C123" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Unspecified</v>
@@ -3762,7 +3806,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C124" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Family</v>
@@ -3777,7 +3821,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C125" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subfamily</v>
@@ -3792,7 +3836,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C126" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Tribe</v>
@@ -3807,7 +3851,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C127" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subtribe</v>
@@ -3822,7 +3866,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C128" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Genus</v>
@@ -3837,7 +3881,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C129" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subgenus</v>
@@ -3852,7 +3896,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="130" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C130" t="str">
         <f t="shared" ref="C130:C193" si="2">D130&amp;"|"&amp;E130</f>
         <v>Mammal|Species</v>
@@ -3867,7 +3911,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="131" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C131" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Subspecies</v>
@@ -3882,7 +3926,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C132" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Variety</v>
@@ -3897,7 +3941,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="133" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C133" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Form</v>
@@ -3912,7 +3956,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="134" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C134" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Race</v>
@@ -3927,7 +3971,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C135" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Stirp</v>
@@ -3942,7 +3986,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="136" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C136" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Morph</v>
@@ -3957,7 +4001,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="137" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C137" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Aberration</v>
@@ -3972,7 +4016,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="138" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C138" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Unspecified</v>
@@ -3987,7 +4031,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="139" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C139" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Family</v>
@@ -4002,7 +4046,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="140" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C140" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subfamily</v>
@@ -4017,7 +4061,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C141" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Tribe</v>
@@ -4032,7 +4076,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="142" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C142" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subtribe</v>
@@ -4047,7 +4091,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C143" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Genus</v>
@@ -4062,7 +4106,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="144" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C144" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subgenus</v>
@@ -4077,7 +4121,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C145" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Section</v>
@@ -4092,7 +4136,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="146" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C146" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subsection</v>
@@ -4107,7 +4151,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="147" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C147" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Species</v>
@@ -4122,7 +4166,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="148" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C148" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subspecies</v>
@@ -4137,7 +4181,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="149" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C149" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Variety</v>
@@ -4152,7 +4196,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="150" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C150" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subvariety</v>
@@ -4167,7 +4211,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="151" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C151" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Form</v>
@@ -4182,7 +4226,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="152" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C152" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subform</v>
@@ -4197,7 +4241,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="153" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C153" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Family</v>
@@ -4212,7 +4256,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="154" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C154" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subfamily</v>
@@ -4227,7 +4271,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C155" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Tribe</v>
@@ -4242,7 +4286,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C156" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subtribe</v>
@@ -4257,7 +4301,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="157" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C157" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Genus</v>
@@ -4272,7 +4316,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="158" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C158" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subgenus</v>
@@ -4287,7 +4331,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C159" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Species</v>
@@ -4302,7 +4346,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="160" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C160" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subspecies</v>
@@ -4317,7 +4361,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C161" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Variety</v>
@@ -4332,7 +4376,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="162" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C162" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Form</v>
@@ -4347,7 +4391,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="163" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C163" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Race</v>
@@ -4362,7 +4406,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="164" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C164" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Stirp</v>
@@ -4377,7 +4421,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="165" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C165" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Morph</v>
@@ -4392,7 +4436,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="166" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C166" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Aberration</v>
@@ -4407,7 +4451,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="167" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C167" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Unspecified</v>
@@ -4422,7 +4466,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="168" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C168" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Family</v>
@@ -4437,7 +4481,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="169" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C169" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subfamily</v>
@@ -4452,7 +4496,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C170" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Tribe</v>
@@ -4467,7 +4511,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="171" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C171" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subtribe</v>
@@ -4482,7 +4526,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C172" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Genus</v>
@@ -4497,7 +4541,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="173" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C173" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subgenus</v>
@@ -4512,7 +4556,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C174" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Species</v>
@@ -4527,7 +4571,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C175" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subspecies</v>
@@ -4542,7 +4586,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="176" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C176" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Unspecified</v>
@@ -4557,7 +4601,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="177" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C177" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Family</v>
@@ -4572,7 +4616,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="178" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C178" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subfamily</v>
@@ -4587,7 +4631,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="179" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C179" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Tribe</v>
@@ -4602,7 +4646,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="180" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C180" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subtribe</v>
@@ -4617,7 +4661,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="181" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C181" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Genus</v>
@@ -4632,7 +4676,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C182" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subgenus</v>
@@ -4647,7 +4691,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="183" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C183" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Species</v>
@@ -4662,7 +4706,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="184" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C184" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subspecies</v>
@@ -4677,7 +4721,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C185" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Variety</v>
@@ -4692,7 +4736,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="186" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C186" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Form</v>
@@ -4707,7 +4751,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C187" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Race</v>
@@ -4722,7 +4766,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="188" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C188" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Stirp</v>
@@ -4737,7 +4781,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="189" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C189" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Morph</v>
@@ -4752,7 +4796,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="190" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C190" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Aberration</v>
@@ -4767,7 +4811,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="191" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C191" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Unspecified</v>
@@ -4782,7 +4826,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="192" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C192" t="str">
         <f t="shared" si="2"/>
         <v>Slug/Snail|Family</v>
@@ -4797,7 +4841,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="193" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C193" t="str">
         <f t="shared" si="2"/>
         <v>Slug/Snail|Subfamily</v>
@@ -4812,7 +4856,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="194" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C194" t="str">
         <f t="shared" ref="C194:C236" si="3">D194&amp;"|"&amp;E194</f>
         <v>Slug/Snail|Tribe</v>
@@ -4827,7 +4871,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="195" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C195" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subtribe</v>
@@ -4842,7 +4886,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C196" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Genus</v>
@@ -4857,7 +4901,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="197" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C197" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subgenus</v>
@@ -4872,7 +4916,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="198" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C198" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Species</v>
@@ -4887,7 +4931,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="199" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C199" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subspecies</v>
@@ -4902,7 +4946,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="200" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C200" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Variety</v>
@@ -4917,7 +4961,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="201" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C201" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Form</v>
@@ -4932,7 +4976,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="202" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C202" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Race</v>
@@ -4947,7 +4991,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="203" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C203" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Stirp</v>
@@ -4962,7 +5006,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="204" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C204" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Morph</v>
@@ -4977,7 +5021,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="205" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C205" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Aberration</v>
@@ -4992,7 +5036,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="206" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C206" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Unspecified</v>
@@ -5007,7 +5051,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="207" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C207" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Family</v>
@@ -5022,7 +5066,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="208" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C208" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subfamily</v>
@@ -5037,7 +5081,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C209" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Tribe</v>
@@ -5052,7 +5096,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="210" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C210" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subtribe</v>
@@ -5067,7 +5111,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="211" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C211" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Genus</v>
@@ -5082,7 +5126,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="212" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C212" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subgenus</v>
@@ -5097,7 +5141,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="213" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C213" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Species</v>
@@ -5112,7 +5156,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="214" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C214" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subspecies</v>
@@ -5127,7 +5171,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="215" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C215" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Variety</v>
@@ -5142,7 +5186,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="216" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C216" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Form</v>
@@ -5157,7 +5201,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="217" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C217" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Race</v>
@@ -5172,7 +5216,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="218" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C218" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Stirp</v>
@@ -5187,7 +5231,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="219" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C219" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Morph</v>
@@ -5202,7 +5246,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="220" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C220" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Aberration</v>
@@ -5217,7 +5261,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="221" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C221" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Unspecified</v>
@@ -5232,7 +5276,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="222" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C222" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Family</v>
@@ -5247,7 +5291,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="223" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C223" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subfamily</v>
@@ -5262,7 +5306,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="224" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C224" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Tribe</v>
@@ -5277,7 +5321,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="225" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C225" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subtribe</v>
@@ -5292,7 +5336,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="226" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C226" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Genus</v>
@@ -5307,7 +5351,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="227" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C227" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subgenus</v>
@@ -5322,7 +5366,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="228" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C228" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Section</v>
@@ -5337,7 +5381,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="229" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C229" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subsection</v>
@@ -5352,7 +5396,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="230" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C230" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Species</v>
@@ -5367,7 +5411,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="231" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C231" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subspecies</v>
@@ -5382,7 +5426,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C232" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Variety</v>
@@ -5397,7 +5441,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="233" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C233" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subvariety</v>
@@ -5412,7 +5456,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="234" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C234" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Form</v>
@@ -5427,7 +5471,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="235" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C235" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subform</v>
@@ -5442,7 +5486,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="236" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C236" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Unspecified</v>
@@ -5464,6 +5508,90 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5472,7 +5600,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5690,91 +5818,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5782,7 +5851,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5799,29 +5868,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Move two species to FWSpecies
Species:
Glocianus punctiger
Chrysomela lapponica
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="18198" windowHeight="4128" tabRatio="358" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="18195" windowHeight="4125" tabRatio="358" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rules of Behavior" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="138">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -442,21 +442,6 @@
     <t>Download Quick Help 9: Understanding Properly Formatted Scientific Names from ServCat to learn how to correctly format the scientific name.</t>
   </si>
   <si>
-    <t>Chrysomela lapponica</t>
-  </si>
-  <si>
-    <t>Chrysomela lapponica Linnaeus, 1758</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Chrysomela&lt;/em&gt; &lt;em&gt;lapponica&lt;/em&gt; Linnaeus, 1758</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Chrysomela&lt;/em&gt; &lt;em&gt;lapponica&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/4459732</t>
-  </si>
-  <si>
     <t>Insect|Species</t>
   </si>
   <si>
@@ -473,18 +458,6 @@
   </si>
   <si>
     <t>https://www.gbif.org/species/8042552</t>
-  </si>
-  <si>
-    <t>Rhynchaenus punctiger Sahlberg, 1835</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Rhynchaenus&lt;/em&gt; &lt;em&gt;punctiger&lt;/em&gt; Sahlberg, 1835</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Rhynchaenus&lt;/em&gt; &lt;em&gt;punctiger&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/1187423</t>
   </si>
   <si>
     <t>Insect|Genus</t>
@@ -1175,97 +1148,97 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="169.578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="169.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>47</v>
       </c>
@@ -1280,32 +1253,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.41796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.26171875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.41796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83984375" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.15625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.15625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.26171875" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.41796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="86.578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="86.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="47" style="12" customWidth="1"/>
-    <col min="14" max="16384" width="8.83984375" style="4"/>
+    <col min="14" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
@@ -1346,15 +1319,15 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>117</v>
@@ -1363,161 +1336,103 @@
         <v>49</v>
       </c>
       <c r="G2" s="12">
-        <v>614016</v>
+        <v>553065</v>
       </c>
       <c r="K2" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="L2" s="12" t="s">
-        <v>118</v>
-      </c>
       <c r="M2" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G3" s="12">
-        <v>553065</v>
+        <v>23502</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L3" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="12">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>127</v>
-      </c>
       <c r="D4" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="12">
-        <v>992283</v>
+      <c r="H4" s="12">
+        <v>4</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G5" s="12">
-        <v>23502</v>
+        <v>1006311</v>
       </c>
       <c r="K5" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M5" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12">
-        <v>5</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="12">
-        <v>4</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="12">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="12">
-        <v>1006311</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1547,7 +1462,7 @@
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
-      <formula1>$A$2:$A$926</formula1>
+      <formula1>$A$2:$A$924</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1582,25 +1497,25 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.41796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.26171875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.41796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.15625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.15625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.26171875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.41796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="86.578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.68359375" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="8.83984375" style="9"/>
+    <col min="2" max="2" width="21.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="86.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
@@ -1641,7 +1556,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43758</v>
       </c>
@@ -1676,7 +1591,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -1703,7 +1618,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1738,7 +1653,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>22</v>
       </c>
@@ -1771,7 +1686,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>23</v>
       </c>
@@ -1804,7 +1719,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>24</v>
       </c>
@@ -1839,7 +1754,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>25</v>
       </c>
@@ -1938,16 +1853,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -1964,7 +1879,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1982,7 +1897,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -2000,7 +1915,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -2018,7 +1933,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2036,7 +1951,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Genus</v>
@@ -2051,7 +1966,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Subgenus</v>
@@ -2066,7 +1981,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Species</v>
@@ -2081,7 +1996,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Subspecies</v>
@@ -2096,7 +2011,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Variety</v>
@@ -2111,7 +2026,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Form</v>
@@ -2126,7 +2041,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Race</v>
@@ -2141,7 +2056,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Stirp</v>
@@ -2156,7 +2071,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Morph</v>
@@ -2171,7 +2086,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Aberration</v>
@@ -2186,7 +2101,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Unspecified</v>
@@ -2201,7 +2116,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Family</v>
@@ -2216,7 +2131,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subfamily</v>
@@ -2231,7 +2146,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Tribe</v>
@@ -2246,7 +2161,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subtribe</v>
@@ -2261,7 +2176,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Genus</v>
@@ -2276,7 +2191,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subgenus</v>
@@ -2291,7 +2206,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Species</v>
@@ -2306,7 +2221,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subspecies</v>
@@ -2321,7 +2236,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Family</v>
@@ -2336,7 +2251,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subfamily</v>
@@ -2351,7 +2266,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Tribe</v>
@@ -2366,7 +2281,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subtribe</v>
@@ -2381,7 +2296,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Genus</v>
@@ -2396,7 +2311,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subgenus</v>
@@ -2411,7 +2326,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Species</v>
@@ -2426,7 +2341,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subspecies</v>
@@ -2441,7 +2356,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Unspecified</v>
@@ -2456,7 +2371,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Family</v>
@@ -2471,7 +2386,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subfamily</v>
@@ -2486,7 +2401,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C36" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Tribe</v>
@@ -2501,7 +2416,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subtribe</v>
@@ -2516,7 +2431,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Genus</v>
@@ -2531,7 +2446,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C39" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subgenus</v>
@@ -2546,7 +2461,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Species</v>
@@ -2561,7 +2476,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subspecies</v>
@@ -2576,7 +2491,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Variety</v>
@@ -2591,7 +2506,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C43" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Form</v>
@@ -2606,7 +2521,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C44" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Race</v>
@@ -2621,7 +2536,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Stirp</v>
@@ -2636,7 +2551,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Morph</v>
@@ -2651,7 +2566,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C47" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Aberration</v>
@@ -2666,7 +2581,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Unspecified</v>
@@ -2681,7 +2596,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Family</v>
@@ -2696,7 +2611,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subfamily</v>
@@ -2711,7 +2626,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C51" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Tribe</v>
@@ -2726,7 +2641,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C52" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subtribe</v>
@@ -2741,7 +2656,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C53" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Genus</v>
@@ -2756,7 +2671,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C54" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subgenus</v>
@@ -2771,7 +2686,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C55" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Section</v>
@@ -2786,7 +2701,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C56" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subsection</v>
@@ -2801,7 +2716,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C57" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Species</v>
@@ -2816,7 +2731,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C58" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subspecies</v>
@@ -2831,7 +2746,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C59" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Variety</v>
@@ -2846,7 +2761,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C60" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subvariety</v>
@@ -2861,7 +2776,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C61" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Form</v>
@@ -2876,7 +2791,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C62" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subform</v>
@@ -2891,7 +2806,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C63" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Unspecified</v>
@@ -2906,7 +2821,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C64" t="str">
         <f t="shared" si="0"/>
         <v>Crab/Lobster/Shrimp|Family</v>
@@ -2921,7 +2836,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" t="str">
         <f t="shared" si="0"/>
         <v>Crab/Lobster/Shrimp|Subfamily</v>
@@ -2936,7 +2851,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" t="str">
         <f t="shared" ref="C66:C129" si="1">D66&amp;"|"&amp;E66</f>
         <v>Crab/Lobster/Shrimp|Tribe</v>
@@ -2951,7 +2866,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subtribe</v>
@@ -2966,7 +2881,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Genus</v>
@@ -2981,7 +2896,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subgenus</v>
@@ -2996,7 +2911,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Species</v>
@@ -3011,7 +2926,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C71" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subspecies</v>
@@ -3026,7 +2941,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C72" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Variety</v>
@@ -3041,7 +2956,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Form</v>
@@ -3056,7 +2971,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Race</v>
@@ -3071,7 +2986,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C75" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Stirp</v>
@@ -3086,7 +3001,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C76" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Morph</v>
@@ -3101,7 +3016,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C77" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Aberration</v>
@@ -3116,7 +3031,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C78" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Unspecified</v>
@@ -3131,7 +3046,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C79" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Family</v>
@@ -3146,7 +3061,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C80" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subfamily</v>
@@ -3161,7 +3076,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C81" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Tribe</v>
@@ -3176,7 +3091,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C82" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subtribe</v>
@@ -3191,7 +3106,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C83" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Genus</v>
@@ -3206,7 +3121,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C84" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subgenus</v>
@@ -3221,7 +3136,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C85" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Species</v>
@@ -3236,7 +3151,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C86" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subspecies</v>
@@ -3251,7 +3166,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C87" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Variety</v>
@@ -3266,7 +3181,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C88" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Form</v>
@@ -3281,7 +3196,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C89" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Race</v>
@@ -3296,7 +3211,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C90" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Stirp</v>
@@ -3311,7 +3226,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C91" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Morph</v>
@@ -3326,7 +3241,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C92" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Aberration</v>
@@ -3341,7 +3256,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C93" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Unspecified</v>
@@ -3356,7 +3271,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C94" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Family</v>
@@ -3371,7 +3286,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C95" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subfamily</v>
@@ -3386,7 +3301,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C96" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Tribe</v>
@@ -3401,7 +3316,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C97" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subtribe</v>
@@ -3416,7 +3331,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C98" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Genus</v>
@@ -3431,7 +3346,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C99" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subgenus</v>
@@ -3446,7 +3361,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C100" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Section</v>
@@ -3461,7 +3376,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C101" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subsection</v>
@@ -3476,7 +3391,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C102" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Species</v>
@@ -3491,7 +3406,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C103" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subspecies</v>
@@ -3506,7 +3421,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C104" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Variety</v>
@@ -3521,7 +3436,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C105" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subvariety</v>
@@ -3536,7 +3451,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C106" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Form</v>
@@ -3551,7 +3466,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C107" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subform</v>
@@ -3566,7 +3481,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C108" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Unspecified</v>
@@ -3581,7 +3496,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C109" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Family</v>
@@ -3596,7 +3511,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C110" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subfamily</v>
@@ -3611,7 +3526,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C111" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Tribe</v>
@@ -3626,7 +3541,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C112" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subtribe</v>
@@ -3641,7 +3556,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C113" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Genus</v>
@@ -3656,7 +3571,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C114" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subgenus</v>
@@ -3671,7 +3586,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C115" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Species</v>
@@ -3686,7 +3601,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C116" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subspecies</v>
@@ -3701,7 +3616,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C117" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Variety</v>
@@ -3716,7 +3631,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C118" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Form</v>
@@ -3731,7 +3646,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C119" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Race</v>
@@ -3746,7 +3661,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C120" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Stirp</v>
@@ -3761,7 +3676,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C121" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Morph</v>
@@ -3776,7 +3691,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C122" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Aberration</v>
@@ -3791,7 +3706,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C123" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Unspecified</v>
@@ -3806,7 +3721,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C124" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Family</v>
@@ -3821,7 +3736,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C125" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subfamily</v>
@@ -3836,7 +3751,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C126" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Tribe</v>
@@ -3851,7 +3766,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C127" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subtribe</v>
@@ -3866,7 +3781,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C128" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Genus</v>
@@ -3881,7 +3796,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C129" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subgenus</v>
@@ -3896,7 +3811,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="130" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C130" t="str">
         <f t="shared" ref="C130:C193" si="2">D130&amp;"|"&amp;E130</f>
         <v>Mammal|Species</v>
@@ -3911,7 +3826,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="131" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C131" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Subspecies</v>
@@ -3926,7 +3841,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C132" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Variety</v>
@@ -3941,7 +3856,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="133" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C133" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Form</v>
@@ -3956,7 +3871,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="134" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C134" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Race</v>
@@ -3971,7 +3886,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C135" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Stirp</v>
@@ -3986,7 +3901,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="136" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C136" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Morph</v>
@@ -4001,7 +3916,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="137" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C137" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Aberration</v>
@@ -4016,7 +3931,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="138" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C138" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Unspecified</v>
@@ -4031,7 +3946,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="139" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C139" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Family</v>
@@ -4046,7 +3961,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="140" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C140" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subfamily</v>
@@ -4061,7 +3976,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C141" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Tribe</v>
@@ -4076,7 +3991,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="142" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C142" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subtribe</v>
@@ -4091,7 +4006,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C143" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Genus</v>
@@ -4106,7 +4021,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="144" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C144" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subgenus</v>
@@ -4121,7 +4036,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C145" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Section</v>
@@ -4136,7 +4051,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="146" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C146" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subsection</v>
@@ -4151,7 +4066,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="147" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C147" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Species</v>
@@ -4166,7 +4081,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="148" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C148" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subspecies</v>
@@ -4181,7 +4096,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="149" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C149" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Variety</v>
@@ -4196,7 +4111,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="150" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C150" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subvariety</v>
@@ -4211,7 +4126,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="151" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C151" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Form</v>
@@ -4226,7 +4141,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="152" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C152" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subform</v>
@@ -4241,7 +4156,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="153" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C153" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Family</v>
@@ -4256,7 +4171,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="154" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C154" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subfamily</v>
@@ -4271,7 +4186,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C155" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Tribe</v>
@@ -4286,7 +4201,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C156" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subtribe</v>
@@ -4301,7 +4216,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="157" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C157" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Genus</v>
@@ -4316,7 +4231,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="158" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C158" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subgenus</v>
@@ -4331,7 +4246,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C159" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Species</v>
@@ -4346,7 +4261,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="160" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C160" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subspecies</v>
@@ -4361,7 +4276,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C161" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Variety</v>
@@ -4376,7 +4291,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="162" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C162" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Form</v>
@@ -4391,7 +4306,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="163" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C163" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Race</v>
@@ -4406,7 +4321,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="164" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C164" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Stirp</v>
@@ -4421,7 +4336,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="165" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C165" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Morph</v>
@@ -4436,7 +4351,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="166" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C166" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Aberration</v>
@@ -4451,7 +4366,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="167" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C167" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Unspecified</v>
@@ -4466,7 +4381,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="168" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C168" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Family</v>
@@ -4481,7 +4396,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="169" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C169" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subfamily</v>
@@ -4496,7 +4411,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C170" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Tribe</v>
@@ -4511,7 +4426,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="171" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C171" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subtribe</v>
@@ -4526,7 +4441,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C172" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Genus</v>
@@ -4541,7 +4456,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="173" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C173" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subgenus</v>
@@ -4556,7 +4471,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C174" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Species</v>
@@ -4571,7 +4486,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C175" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subspecies</v>
@@ -4586,7 +4501,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="176" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C176" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Unspecified</v>
@@ -4601,7 +4516,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="177" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C177" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Family</v>
@@ -4616,7 +4531,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="178" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C178" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subfamily</v>
@@ -4631,7 +4546,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="179" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C179" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Tribe</v>
@@ -4646,7 +4561,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="180" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C180" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subtribe</v>
@@ -4661,7 +4576,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="181" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C181" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Genus</v>
@@ -4676,7 +4591,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C182" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subgenus</v>
@@ -4691,7 +4606,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="183" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C183" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Species</v>
@@ -4706,7 +4621,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="184" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C184" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subspecies</v>
@@ -4721,7 +4636,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C185" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Variety</v>
@@ -4736,7 +4651,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="186" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C186" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Form</v>
@@ -4751,7 +4666,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C187" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Race</v>
@@ -4766,7 +4681,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="188" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C188" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Stirp</v>
@@ -4781,7 +4696,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="189" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C189" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Morph</v>
@@ -4796,7 +4711,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="190" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C190" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Aberration</v>
@@ -4811,7 +4726,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="191" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C191" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Unspecified</v>
@@ -4826,7 +4741,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="192" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C192" t="str">
         <f t="shared" si="2"/>
         <v>Slug/Snail|Family</v>
@@ -4841,7 +4756,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="193" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C193" t="str">
         <f t="shared" si="2"/>
         <v>Slug/Snail|Subfamily</v>
@@ -4856,7 +4771,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="194" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C194" t="str">
         <f t="shared" ref="C194:C236" si="3">D194&amp;"|"&amp;E194</f>
         <v>Slug/Snail|Tribe</v>
@@ -4871,7 +4786,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="195" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C195" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subtribe</v>
@@ -4886,7 +4801,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C196" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Genus</v>
@@ -4901,7 +4816,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="197" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C197" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subgenus</v>
@@ -4916,7 +4831,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="198" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C198" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Species</v>
@@ -4931,7 +4846,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="199" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C199" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subspecies</v>
@@ -4946,7 +4861,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="200" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C200" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Variety</v>
@@ -4961,7 +4876,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="201" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C201" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Form</v>
@@ -4976,7 +4891,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="202" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C202" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Race</v>
@@ -4991,7 +4906,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="203" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C203" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Stirp</v>
@@ -5006,7 +4921,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="204" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C204" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Morph</v>
@@ -5021,7 +4936,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="205" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C205" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Aberration</v>
@@ -5036,7 +4951,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="206" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C206" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Unspecified</v>
@@ -5051,7 +4966,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="207" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C207" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Family</v>
@@ -5066,7 +4981,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="208" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C208" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subfamily</v>
@@ -5081,7 +4996,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C209" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Tribe</v>
@@ -5096,7 +5011,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="210" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C210" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subtribe</v>
@@ -5111,7 +5026,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="211" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C211" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Genus</v>
@@ -5126,7 +5041,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="212" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C212" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subgenus</v>
@@ -5141,7 +5056,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="213" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C213" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Species</v>
@@ -5156,7 +5071,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="214" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C214" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subspecies</v>
@@ -5171,7 +5086,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="215" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C215" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Variety</v>
@@ -5186,7 +5101,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="216" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C216" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Form</v>
@@ -5201,7 +5116,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="217" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C217" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Race</v>
@@ -5216,7 +5131,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="218" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C218" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Stirp</v>
@@ -5231,7 +5146,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="219" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C219" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Morph</v>
@@ -5246,7 +5161,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="220" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C220" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Aberration</v>
@@ -5261,7 +5176,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="221" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C221" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Unspecified</v>
@@ -5276,7 +5191,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="222" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C222" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Family</v>
@@ -5291,7 +5206,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="223" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C223" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subfamily</v>
@@ -5306,7 +5221,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="224" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C224" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Tribe</v>
@@ -5321,7 +5236,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="225" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C225" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subtribe</v>
@@ -5336,7 +5251,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="226" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C226" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Genus</v>
@@ -5351,7 +5266,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="227" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C227" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subgenus</v>
@@ -5366,7 +5281,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="228" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C228" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Section</v>
@@ -5381,7 +5296,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="229" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C229" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subsection</v>
@@ -5396,7 +5311,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="230" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C230" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Species</v>
@@ -5411,7 +5326,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="231" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C231" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subspecies</v>
@@ -5426,7 +5341,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C232" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Variety</v>
@@ -5441,7 +5356,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="233" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C233" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subvariety</v>
@@ -5456,7 +5371,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="234" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C234" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Form</v>
@@ -5471,7 +5386,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="235" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C235" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subform</v>
@@ -5486,7 +5401,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="236" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C236" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Unspecified</v>

</xml_diff>

<commit_message>
Add several species to Kenai NWR's checklist
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="18195" windowHeight="4125" tabRatio="358" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="108" windowWidth="18198" windowHeight="4128" tabRatio="358" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rules of Behavior" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="116">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -440,54 +440,6 @@
   </si>
   <si>
     <t>Download Quick Help 9: Understanding Properly Formatted Scientific Names from ServCat to learn how to correctly format the scientific name.</t>
-  </si>
-  <si>
-    <t>Cortinarius lucorum (Fr.) Berger, 1846</t>
-  </si>
-  <si>
-    <t>Cortinarius lucorum</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Cortinarius&lt;/em&gt; &lt;em&gt;lucorum&lt;/em&gt; (Fr.) Berger, 1846</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;em&gt;Cortinarius&lt;/em&gt; &lt;em&gt;lucorum&lt;/em&gt; </t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/9695037</t>
-  </si>
-  <si>
-    <t>Insect|Species</t>
-  </si>
-  <si>
-    <t>Corticarina minuta</t>
-  </si>
-  <si>
-    <t>Corticarina minuta (Fabricius, 1792)</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Corticarina&lt;/em&gt; &lt;em&gt;minuta&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Corticarina&lt;/em&gt; &lt;em&gt;minuta&lt;/em&gt; (Fabricius, 1792)</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/4450799</t>
-  </si>
-  <si>
-    <t>Stephostethus armatulus</t>
-  </si>
-  <si>
-    <t>Stephostethus armatulus (Fall, 1899)</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Stephostethus&lt;/em&gt; &lt;em&gt;armatulus&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Stephostethus&lt;/em&gt; &lt;em&gt;armatulus&lt;/em&gt; (Fall, 1899)</t>
-  </si>
-  <si>
-    <t>http://www.latridiidae.de/index_htm_files/Checkliste%20LATRIDIIDAE.pdf</t>
   </si>
 </sst>
 </file>
@@ -1130,97 +1082,97 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="169.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="169.578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
         <v>47</v>
       </c>
@@ -1235,32 +1187,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="86.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.41796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.26171875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.41796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.15625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.15625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.26171875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.41796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="86.578125" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="47" style="12" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="4"/>
+    <col min="14" max="16384" width="8.83984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
@@ -1299,84 +1251,6 @@
       </c>
       <c r="M1" s="11" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="12">
-        <v>668590</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="12">
-        <v>560720</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" s="12">
-        <v>559164</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1390,6 +1264,10 @@
     <cfRule type="duplicateValues" dxfId="4" priority="9"/>
   </conditionalFormatting>
   <dataValidations count="5">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sci. Name w/auth. text" error="Scientific Name with Authority must be text between 3 and 175 characters in length." sqref="D1:D1048576">
+      <formula1>3</formula1>
+      <formula2>175</formula2>
+    </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Positive Integers only" error="Only positive integers are allowed in the ID column." sqref="A1:A1048576">
       <formula1>1</formula1>
       <formula2>63000</formula2>
@@ -1398,15 +1276,11 @@
       <formula1>2</formula1>
       <formula2>87</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sci. Name w/auth. text" error="Scientific Name with Authority must be text between 3 and 175 characters in length." sqref="D1 D2:D1048576">
-      <formula1>3</formula1>
-      <formula2>175</formula2>
-    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
-      <formula1>$A$2:$A$927</formula1>
+      <formula1>$A$2:$A$924</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1441,25 +1315,25 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="86.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="9"/>
+    <col min="2" max="2" width="21.578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.41796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.26171875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.41796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.15625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.15625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.26171875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.41796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="86.578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.68359375" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="8.83984375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
@@ -1500,7 +1374,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7">
         <v>43758</v>
       </c>
@@ -1535,7 +1409,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -1562,7 +1436,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1597,7 +1471,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7">
         <v>22</v>
       </c>
@@ -1630,7 +1504,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8">
         <v>23</v>
       </c>
@@ -1663,7 +1537,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8">
         <v>24</v>
       </c>
@@ -1698,7 +1572,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8">
         <v>25</v>
       </c>
@@ -1797,16 +1671,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -1823,7 +1697,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1841,7 +1715,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1859,7 +1733,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1877,7 +1751,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1895,7 +1769,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Genus</v>
@@ -1910,7 +1784,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Subgenus</v>
@@ -1925,7 +1799,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Species</v>
@@ -1940,7 +1814,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Subspecies</v>
@@ -1955,7 +1829,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Variety</v>
@@ -1970,7 +1844,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Form</v>
@@ -1985,7 +1859,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Race</v>
@@ -2000,7 +1874,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Stirp</v>
@@ -2015,7 +1889,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Morph</v>
@@ -2030,7 +1904,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Aberration</v>
@@ -2045,7 +1919,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>Amphibian|Unspecified</v>
@@ -2060,7 +1934,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Family</v>
@@ -2075,7 +1949,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subfamily</v>
@@ -2090,7 +1964,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Tribe</v>
@@ -2105,7 +1979,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subtribe</v>
@@ -2120,7 +1994,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Genus</v>
@@ -2135,7 +2009,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subgenus</v>
@@ -2150,7 +2024,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Species</v>
@@ -2165,7 +2039,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>Archaea|Subspecies</v>
@@ -2180,7 +2054,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Family</v>
@@ -2195,7 +2069,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subfamily</v>
@@ -2210,7 +2084,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Tribe</v>
@@ -2225,7 +2099,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subtribe</v>
@@ -2240,7 +2114,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Genus</v>
@@ -2255,7 +2129,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subgenus</v>
@@ -2270,7 +2144,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Species</v>
@@ -2285,7 +2159,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Subspecies</v>
@@ -2300,7 +2174,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria|Unspecified</v>
@@ -2315,7 +2189,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Family</v>
@@ -2330,7 +2204,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subfamily</v>
@@ -2345,7 +2219,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C36" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Tribe</v>
@@ -2360,7 +2234,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C37" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subtribe</v>
@@ -2375,7 +2249,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Genus</v>
@@ -2390,7 +2264,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subgenus</v>
@@ -2405,7 +2279,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C40" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Species</v>
@@ -2420,7 +2294,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C41" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Subspecies</v>
@@ -2435,7 +2309,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Variety</v>
@@ -2450,7 +2324,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Form</v>
@@ -2465,7 +2339,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C44" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Race</v>
@@ -2480,7 +2354,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Stirp</v>
@@ -2495,7 +2369,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Morph</v>
@@ -2510,7 +2384,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C47" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Aberration</v>
@@ -2525,7 +2399,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" t="str">
         <f t="shared" si="0"/>
         <v>Bird|Unspecified</v>
@@ -2540,7 +2414,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Family</v>
@@ -2555,7 +2429,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C50" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subfamily</v>
@@ -2570,7 +2444,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C51" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Tribe</v>
@@ -2585,7 +2459,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C52" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subtribe</v>
@@ -2600,7 +2474,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C53" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Genus</v>
@@ -2615,7 +2489,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C54" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subgenus</v>
@@ -2630,7 +2504,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C55" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Section</v>
@@ -2645,7 +2519,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C56" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subsection</v>
@@ -2660,7 +2534,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C57" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Species</v>
@@ -2675,7 +2549,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C58" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subspecies</v>
@@ -2690,7 +2564,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C59" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Variety</v>
@@ -2705,7 +2579,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C60" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subvariety</v>
@@ -2720,7 +2594,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C61" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Form</v>
@@ -2735,7 +2609,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C62" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Subform</v>
@@ -2750,7 +2624,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C63" t="str">
         <f t="shared" si="0"/>
         <v>Chromista|Unspecified</v>
@@ -2765,7 +2639,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" t="str">
         <f t="shared" si="0"/>
         <v>Crab/Lobster/Shrimp|Family</v>
@@ -2780,7 +2654,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C65" t="str">
         <f t="shared" si="0"/>
         <v>Crab/Lobster/Shrimp|Subfamily</v>
@@ -2795,7 +2669,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C66" t="str">
         <f t="shared" ref="C66:C129" si="1">D66&amp;"|"&amp;E66</f>
         <v>Crab/Lobster/Shrimp|Tribe</v>
@@ -2810,7 +2684,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subtribe</v>
@@ -2825,7 +2699,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Genus</v>
@@ -2840,7 +2714,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subgenus</v>
@@ -2855,7 +2729,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Species</v>
@@ -2870,7 +2744,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C71" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Subspecies</v>
@@ -2885,7 +2759,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C72" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Variety</v>
@@ -2900,7 +2774,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C73" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Form</v>
@@ -2915,7 +2789,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C74" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Race</v>
@@ -2930,7 +2804,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C75" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Stirp</v>
@@ -2945,7 +2819,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C76" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Morph</v>
@@ -2960,7 +2834,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C77" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Aberration</v>
@@ -2975,7 +2849,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C78" t="str">
         <f t="shared" si="1"/>
         <v>Crab/Lobster/Shrimp|Unspecified</v>
@@ -2990,7 +2864,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C79" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Family</v>
@@ -3005,7 +2879,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C80" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subfamily</v>
@@ -3020,7 +2894,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C81" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Tribe</v>
@@ -3035,7 +2909,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C82" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subtribe</v>
@@ -3050,7 +2924,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C83" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Genus</v>
@@ -3065,7 +2939,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C84" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subgenus</v>
@@ -3080,7 +2954,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C85" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Species</v>
@@ -3095,7 +2969,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C86" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Subspecies</v>
@@ -3110,7 +2984,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C87" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Variety</v>
@@ -3125,7 +2999,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C88" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Form</v>
@@ -3140,7 +3014,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C89" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Race</v>
@@ -3155,7 +3029,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C90" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Stirp</v>
@@ -3170,7 +3044,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C91" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Morph</v>
@@ -3185,7 +3059,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C92" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Aberration</v>
@@ -3200,7 +3074,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C93" t="str">
         <f t="shared" si="1"/>
         <v>Fish|Unspecified</v>
@@ -3215,7 +3089,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C94" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Family</v>
@@ -3230,7 +3104,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C95" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subfamily</v>
@@ -3245,7 +3119,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C96" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Tribe</v>
@@ -3260,7 +3134,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C97" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subtribe</v>
@@ -3275,7 +3149,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C98" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Genus</v>
@@ -3290,7 +3164,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C99" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subgenus</v>
@@ -3305,7 +3179,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C100" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Section</v>
@@ -3320,7 +3194,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C101" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subsection</v>
@@ -3335,7 +3209,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C102" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Species</v>
@@ -3350,7 +3224,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C103" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subspecies</v>
@@ -3365,7 +3239,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C104" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Variety</v>
@@ -3380,7 +3254,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C105" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subvariety</v>
@@ -3395,7 +3269,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C106" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Form</v>
@@ -3410,7 +3284,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C107" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Subform</v>
@@ -3425,7 +3299,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C108" t="str">
         <f t="shared" si="1"/>
         <v>Fungi|Unspecified</v>
@@ -3440,7 +3314,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C109" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Family</v>
@@ -3455,7 +3329,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C110" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subfamily</v>
@@ -3470,7 +3344,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C111" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Tribe</v>
@@ -3485,7 +3359,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C112" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subtribe</v>
@@ -3500,7 +3374,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C113" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Genus</v>
@@ -3515,7 +3389,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C114" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subgenus</v>
@@ -3530,7 +3404,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C115" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Species</v>
@@ -3545,7 +3419,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C116" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Subspecies</v>
@@ -3560,7 +3434,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C117" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Variety</v>
@@ -3575,7 +3449,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C118" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Form</v>
@@ -3590,7 +3464,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C119" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Race</v>
@@ -3605,7 +3479,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C120" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Stirp</v>
@@ -3620,7 +3494,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C121" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Morph</v>
@@ -3635,7 +3509,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C122" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Aberration</v>
@@ -3650,7 +3524,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C123" t="str">
         <f t="shared" si="1"/>
         <v>Insect|Unspecified</v>
@@ -3665,7 +3539,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C124" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Family</v>
@@ -3680,7 +3554,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C125" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subfamily</v>
@@ -3695,7 +3569,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C126" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Tribe</v>
@@ -3710,7 +3584,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C127" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subtribe</v>
@@ -3725,7 +3599,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C128" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Genus</v>
@@ -3740,7 +3614,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C129" t="str">
         <f t="shared" si="1"/>
         <v>Mammal|Subgenus</v>
@@ -3755,7 +3629,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="130" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C130" t="str">
         <f t="shared" ref="C130:C193" si="2">D130&amp;"|"&amp;E130</f>
         <v>Mammal|Species</v>
@@ -3770,7 +3644,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="131" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C131" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Subspecies</v>
@@ -3785,7 +3659,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C132" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Variety</v>
@@ -3800,7 +3674,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="133" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C133" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Form</v>
@@ -3815,7 +3689,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="134" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C134" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Race</v>
@@ -3830,7 +3704,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C135" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Stirp</v>
@@ -3845,7 +3719,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="136" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C136" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Morph</v>
@@ -3860,7 +3734,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="137" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C137" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Aberration</v>
@@ -3875,7 +3749,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="138" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C138" t="str">
         <f t="shared" si="2"/>
         <v>Mammal|Unspecified</v>
@@ -3890,7 +3764,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="139" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C139" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Family</v>
@@ -3905,7 +3779,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="140" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C140" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subfamily</v>
@@ -3920,7 +3794,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C141" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Tribe</v>
@@ -3935,7 +3809,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="142" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C142" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subtribe</v>
@@ -3950,7 +3824,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C143" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Genus</v>
@@ -3965,7 +3839,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="144" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C144" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subgenus</v>
@@ -3980,7 +3854,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C145" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Section</v>
@@ -3995,7 +3869,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="146" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C146" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subsection</v>
@@ -4010,7 +3884,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="147" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C147" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Species</v>
@@ -4025,7 +3899,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="148" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C148" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subspecies</v>
@@ -4040,7 +3914,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="149" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C149" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Variety</v>
@@ -4055,7 +3929,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="150" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C150" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subvariety</v>
@@ -4070,7 +3944,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="151" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C151" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Form</v>
@@ -4085,7 +3959,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="152" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C152" t="str">
         <f t="shared" si="2"/>
         <v>Non-vascular Plant|Subform</v>
@@ -4100,7 +3974,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="153" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C153" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Family</v>
@@ -4115,7 +3989,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="154" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C154" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subfamily</v>
@@ -4130,7 +4004,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C155" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Tribe</v>
@@ -4145,7 +4019,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C156" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subtribe</v>
@@ -4160,7 +4034,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="157" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C157" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Genus</v>
@@ -4175,7 +4049,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="158" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C158" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subgenus</v>
@@ -4190,7 +4064,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C159" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Species</v>
@@ -4205,7 +4079,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="160" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C160" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Subspecies</v>
@@ -4220,7 +4094,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C161" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Variety</v>
@@ -4235,7 +4109,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="162" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C162" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Form</v>
@@ -4250,7 +4124,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="163" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C163" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Race</v>
@@ -4265,7 +4139,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="164" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C164" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Stirp</v>
@@ -4280,7 +4154,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="165" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C165" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Morph</v>
@@ -4295,7 +4169,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="166" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C166" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Aberration</v>
@@ -4310,7 +4184,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="167" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C167" t="str">
         <f t="shared" si="2"/>
         <v>Other Non-vertebrates|Unspecified</v>
@@ -4325,7 +4199,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="168" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C168" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Family</v>
@@ -4340,7 +4214,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="169" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C169" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subfamily</v>
@@ -4355,7 +4229,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C170" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Tribe</v>
@@ -4370,7 +4244,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="171" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C171" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subtribe</v>
@@ -4385,7 +4259,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C172" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Genus</v>
@@ -4400,7 +4274,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="173" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C173" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subgenus</v>
@@ -4415,7 +4289,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C174" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Species</v>
@@ -4430,7 +4304,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C175" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Subspecies</v>
@@ -4445,7 +4319,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="176" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C176" t="str">
         <f t="shared" si="2"/>
         <v>Protozoa|Unspecified</v>
@@ -4460,7 +4334,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="177" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C177" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Family</v>
@@ -4475,7 +4349,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="178" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C178" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subfamily</v>
@@ -4490,7 +4364,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="179" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C179" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Tribe</v>
@@ -4505,7 +4379,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="180" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C180" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subtribe</v>
@@ -4520,7 +4394,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="181" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C181" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Genus</v>
@@ -4535,7 +4409,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C182" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subgenus</v>
@@ -4550,7 +4424,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="183" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C183" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Species</v>
@@ -4565,7 +4439,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="184" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C184" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Subspecies</v>
@@ -4580,7 +4454,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C185" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Variety</v>
@@ -4595,7 +4469,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="186" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C186" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Form</v>
@@ -4610,7 +4484,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C187" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Race</v>
@@ -4625,7 +4499,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="188" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C188" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Stirp</v>
@@ -4640,7 +4514,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="189" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C189" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Morph</v>
@@ -4655,7 +4529,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="190" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C190" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Aberration</v>
@@ -4670,7 +4544,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="191" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C191" t="str">
         <f t="shared" si="2"/>
         <v>Reptile|Unspecified</v>
@@ -4685,7 +4559,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="192" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C192" t="str">
         <f t="shared" si="2"/>
         <v>Slug/Snail|Family</v>
@@ -4700,7 +4574,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="193" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C193" t="str">
         <f t="shared" si="2"/>
         <v>Slug/Snail|Subfamily</v>
@@ -4715,7 +4589,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="194" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C194" t="str">
         <f t="shared" ref="C194:C236" si="3">D194&amp;"|"&amp;E194</f>
         <v>Slug/Snail|Tribe</v>
@@ -4730,7 +4604,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="195" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C195" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subtribe</v>
@@ -4745,7 +4619,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C196" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Genus</v>
@@ -4760,7 +4634,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="197" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C197" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subgenus</v>
@@ -4775,7 +4649,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="198" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C198" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Species</v>
@@ -4790,7 +4664,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="199" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C199" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Subspecies</v>
@@ -4805,7 +4679,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="200" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C200" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Variety</v>
@@ -4820,7 +4694,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="201" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C201" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Form</v>
@@ -4835,7 +4709,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="202" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C202" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Race</v>
@@ -4850,7 +4724,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="203" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C203" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Stirp</v>
@@ -4865,7 +4739,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="204" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C204" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Morph</v>
@@ -4880,7 +4754,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="205" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C205" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Aberration</v>
@@ -4895,7 +4769,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="206" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C206" t="str">
         <f t="shared" si="3"/>
         <v>Slug/Snail|Unspecified</v>
@@ -4910,7 +4784,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="207" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C207" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Family</v>
@@ -4925,7 +4799,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="208" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C208" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subfamily</v>
@@ -4940,7 +4814,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C209" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Tribe</v>
@@ -4955,7 +4829,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="210" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C210" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subtribe</v>
@@ -4970,7 +4844,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="211" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C211" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Genus</v>
@@ -4985,7 +4859,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="212" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C212" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subgenus</v>
@@ -5000,7 +4874,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="213" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C213" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Species</v>
@@ -5015,7 +4889,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="214" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C214" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Subspecies</v>
@@ -5030,7 +4904,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="215" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C215" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Variety</v>
@@ -5045,7 +4919,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="216" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C216" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Form</v>
@@ -5060,7 +4934,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="217" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C217" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Race</v>
@@ -5075,7 +4949,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="218" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C218" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Stirp</v>
@@ -5090,7 +4964,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="219" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C219" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Morph</v>
@@ -5105,7 +4979,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="220" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C220" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Aberration</v>
@@ -5120,7 +4994,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="221" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C221" t="str">
         <f t="shared" si="3"/>
         <v>Spider/Scorpion|Unspecified</v>
@@ -5135,7 +5009,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="222" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C222" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Family</v>
@@ -5150,7 +5024,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="223" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C223" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subfamily</v>
@@ -5165,7 +5039,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="224" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C224" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Tribe</v>
@@ -5180,7 +5054,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="225" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C225" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subtribe</v>
@@ -5195,7 +5069,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="226" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C226" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Genus</v>
@@ -5210,7 +5084,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="227" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C227" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subgenus</v>
@@ -5225,7 +5099,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="228" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C228" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Section</v>
@@ -5240,7 +5114,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="229" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C229" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subsection</v>
@@ -5255,7 +5129,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="230" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C230" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Species</v>
@@ -5270,7 +5144,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="231" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C231" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subspecies</v>
@@ -5285,7 +5159,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C232" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Variety</v>
@@ -5300,7 +5174,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="233" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C233" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subvariety</v>
@@ -5315,7 +5189,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="234" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C234" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Form</v>
@@ -5330,7 +5204,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="235" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C235" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Subform</v>
@@ -5345,7 +5219,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="236" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C236" t="str">
         <f t="shared" si="3"/>
         <v>Vascular Plant|Unspecified</v>
@@ -5367,44 +5241,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5622,16 +5458,45 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5677,24 +5542,16 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5713,18 +5570,35 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update a few species records
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="122">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -440,6 +440,24 @@
   </si>
   <si>
     <t>Download Quick Help 9: Understanding Properly Formatted Scientific Names from ServCat to learn how to correctly format the scientific name.</t>
+  </si>
+  <si>
+    <t>Acidota quadrata</t>
+  </si>
+  <si>
+    <t>Acidota quadrata (Zetterstedt, 1838)</t>
+  </si>
+  <si>
+    <t>Insect|Species</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Acidota&lt;/em&gt; &lt;em&gt;quadrata&lt;/em&gt; (Zetterstedt, 1838)</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Acidota&lt;/em&gt; &lt;em&gt;quadrata&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/4444228</t>
   </si>
 </sst>
 </file>
@@ -1187,11 +1205,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1251,6 +1269,32 @@
       </c>
       <c r="M1" s="11" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -5241,6 +5285,99 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5458,100 +5595,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5568,37 +5645,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Move species to FWSpecies
Moved:
Acidota quadratum
Anaspis rufa
Eucnecosum brachypterum
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -442,22 +442,22 @@
     <t>Download Quick Help 9: Understanding Properly Formatted Scientific Names from ServCat to learn how to correctly format the scientific name.</t>
   </si>
   <si>
-    <t>Acidota quadrata</t>
-  </si>
-  <si>
-    <t>Acidota quadrata (Zetterstedt, 1838)</t>
-  </si>
-  <si>
     <t>Insect|Species</t>
   </si>
   <si>
-    <t>&lt;em&gt;Acidota&lt;/em&gt; &lt;em&gt;quadrata&lt;/em&gt; (Zetterstedt, 1838)</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Acidota&lt;/em&gt; &lt;em&gt;quadrata&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/4444228</t>
+    <t>Dinaraea pacei</t>
+  </si>
+  <si>
+    <t>Dinaraea pacei Klimaszewski &amp; Langor, 2011</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Dinaraea&lt;/em&gt; &lt;em&gt;pacei&lt;/em&gt; Klimaszewski &amp; Langor, 2011</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Dinaraea&lt;/em&gt; &lt;em&gt;pacei&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/7971622</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1209,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1276,16 +1276,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>51</v>
+      </c>
+      <c r="G2" s="12">
+        <v>627969</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>120</v>
@@ -1324,7 +1327,7 @@
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
-      <formula1>$A$2:$A$924</formula1>
+      <formula1>$A$2:$A$923</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Move Upis ceramboides to FWSpecies
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="132">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -458,6 +458,36 @@
   </si>
   <si>
     <t>https://www.gbif.org/species/7971622</t>
+  </si>
+  <si>
+    <t>Ostoma fraterna Randall, 1838</t>
+  </si>
+  <si>
+    <t>Ostoma fraterna</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;fraterna&lt;/em&gt; Randall, 1838</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;fraterna&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/9460210</t>
+  </si>
+  <si>
+    <t>https://zookeys.pensoft.net/article/3109/</t>
+  </si>
+  <si>
+    <t>Ostoma septentrionalis</t>
+  </si>
+  <si>
+    <t>Ostoma septentrionalis Randall, 1838</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;septentrionalis&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;septentrionalis&lt;/em&gt; Randall, 1838</t>
   </si>
 </sst>
 </file>
@@ -1205,11 +1235,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1298,6 +1328,64 @@
       </c>
       <c r="M2" s="12" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="12">
+        <v>555212</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="12">
+        <v>555212</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -5289,15 +5377,6 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
     <Name>Document ID Generator</Name>
@@ -5342,45 +5421,16 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5598,7 +5648,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5606,32 +5702,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5648,4 +5719,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add species to FWSpecies' taxonomy
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="142">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -488,6 +488,36 @@
   </si>
   <si>
     <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;septentrionalis&lt;/em&gt; Randall, 1838</t>
+  </si>
+  <si>
+    <t>Liriomyza equiseti De Meijere, 1924</t>
+  </si>
+  <si>
+    <t>Liriomyza equiseti</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Liriomyza&lt;/em&gt; &lt;em&gt;equiseti&lt;/em&gt; De Meijere, 1924</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Liriomyza&lt;/em&gt; &lt;em&gt;equiseti&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/1553334</t>
+  </si>
+  <si>
+    <t>Chirosia similata (Tiensuu, 1939)</t>
+  </si>
+  <si>
+    <t>Chirosia similata</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Chirosia&lt;/em&gt; &lt;em&gt;similata&lt;/em&gt; (Tiensuu, 1939)</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Chirosia&lt;/em&gt; &lt;em&gt;similata&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/1575323</t>
   </si>
 </sst>
 </file>
@@ -1235,11 +1265,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1386,6 +1416,64 @@
       </c>
       <c r="M4" s="12" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="12">
+        <v>49281</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="12">
+        <v>56467</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5376,6 +5464,44 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5421,7 +5547,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5430,7 +5556,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5648,45 +5774,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -5694,7 +5799,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5702,7 +5807,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5719,21 +5824,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Hesperinus brevifrons to FWSpecies
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="147">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -518,6 +518,21 @@
   </si>
   <si>
     <t>https://www.gbif.org/species/1575323</t>
+  </si>
+  <si>
+    <t>Anthomyza gilviventris Roháček &amp; Barber, 2016</t>
+  </si>
+  <si>
+    <t>Anthomyza gilviventris</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Anthomyza&lt;/em&gt; &lt;em&gt;gilviventris&lt;/em&gt; Roháček &amp; Barber, 2016</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Anthomyza&lt;/em&gt; &lt;em&gt;gilviventris&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/312084641_Nearctic_Anthomyzidae_a_monograph_of_Anthomyza_and_allied_genera_Diptera</t>
   </si>
 </sst>
 </file>
@@ -690,7 +705,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -718,6 +733,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1265,18 +1290,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.20703125" style="12" customWidth="1"/>
     <col min="4" max="4" width="33.41796875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.26171875" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.41796875" style="12" bestFit="1" customWidth="1"/>
@@ -1476,18 +1501,50 @@
         <v>141</v>
       </c>
     </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="12">
+        <v>42303</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="9"/>
+  <conditionalFormatting sqref="C1:C6 C8:C1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sci. Name w/auth. text" error="Scientific Name with Authority must be text between 3 and 175 characters in length." sqref="D1:D1048576">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sci. Name w/auth. text" error="Scientific Name with Authority must be text between 3 and 175 characters in length." sqref="D1:D1048576 C7">
       <formula1>3</formula1>
       <formula2>175</formula2>
     </dataValidation>
@@ -1495,7 +1552,7 @@
       <formula1>1</formula1>
       <formula2>63000</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Scientific Name text" error="Scientific Name must be text between 2 and 87 characters in length." sqref="C1:C1048576">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Scientific Name text" error="Scientific Name must be text between 2 and 87 characters in length." sqref="C1:C6 C8:C1048576">
       <formula1>2</formula1>
       <formula2>87</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add taxa to FWSpecies
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="184">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -533,6 +533,117 @@
   </si>
   <si>
     <t>https://www.researchgate.net/publication/312084641_Nearctic_Anthomyzidae_a_monograph_of_Anthomyza_and_allied_genera_Diptera</t>
+  </si>
+  <si>
+    <t>Lirula macrospora</t>
+  </si>
+  <si>
+    <t>Lirula macrospora (R.Hartig) Darker</t>
+  </si>
+  <si>
+    <t>Lirula needle blight</t>
+  </si>
+  <si>
+    <t>Lirula</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Lirula&lt;/em&gt; &lt;em&gt;macrospora&lt;/em&gt; (R.Hartig) Darker</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Lirula&lt;/em&gt; &lt;em&gt;macrospora&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/2579903</t>
+  </si>
+  <si>
+    <t>Lirula Darker</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/2579890</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Lirula&lt;/em&gt; Darker</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Lirula&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Epipyxis gracilis</t>
+  </si>
+  <si>
+    <t>Epipyxis kenaiensis</t>
+  </si>
+  <si>
+    <t>Epipyxis planctonica</t>
+  </si>
+  <si>
+    <t>Epipyxis polymorpha</t>
+  </si>
+  <si>
+    <t>Synura petersenii</t>
+  </si>
+  <si>
+    <t>Synura petersenii Korshikov</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/3195206</t>
+  </si>
+  <si>
+    <t>Chromista|Species</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Synura&lt;/em&gt; &lt;em&gt;petersenii&lt;/em&gt; Korshikov</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Synura&lt;/em&gt; &lt;em&gt;petersenii&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Epipyxis gracilis D.K.Hilliard &amp; Asmund</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/3195021</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;gracilis&lt;/em&gt; D.K.Hilliard &amp; Asmund</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;kenaiensis&lt;/em&gt; D.K.Hilliard &amp; Asmund</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;gracilis&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Epipyxis kenaiensis D.K.Hilliard &amp; Asmund</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;kenaiensis&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/3195033</t>
+  </si>
+  <si>
+    <t>https://www.algaebase.org/search/species/detail/?species_id=112127</t>
+  </si>
+  <si>
+    <t>Epipyxis planctonica D.K.Hilliard &amp; B.C.Asmund</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;planctonica&lt;/em&gt; D.K.Hilliard &amp; B.C.Asmund</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;planctonica&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Epipyxis polymorpha (J.W.G.Lund) D.K.Hilliard &amp; Asmund</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;polymorpha&lt;/em&gt; (J.W.G.Lund) D.K.Hilliard &amp; Asmund</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;polymorpha&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/3195019</t>
   </si>
 </sst>
 </file>
@@ -1290,11 +1401,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1528,6 +1639,212 @@
       </c>
       <c r="M7" s="12" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="12">
+        <v>8</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="12">
+        <v>388655</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="12">
+        <v>63440</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="12">
+        <v>63440</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="12">
+        <v>63440</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="12">
+        <v>63440</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="12">
+        <v>68346</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submit new taxonomy additions
</commit_message>
<xml_diff>
--- a/data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="148">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -445,205 +445,97 @@
     <t>Insect|Species</t>
   </si>
   <si>
-    <t>Dinaraea pacei</t>
-  </si>
-  <si>
-    <t>Dinaraea pacei Klimaszewski &amp; Langor, 2011</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Dinaraea&lt;/em&gt; &lt;em&gt;pacei&lt;/em&gt; Klimaszewski &amp; Langor, 2011</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Dinaraea&lt;/em&gt; &lt;em&gt;pacei&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/7971622</t>
-  </si>
-  <si>
-    <t>Ostoma fraterna Randall, 1838</t>
-  </si>
-  <si>
-    <t>Ostoma fraterna</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;fraterna&lt;/em&gt; Randall, 1838</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;fraterna&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/9460210</t>
-  </si>
-  <si>
-    <t>https://zookeys.pensoft.net/article/3109/</t>
-  </si>
-  <si>
-    <t>Ostoma septentrionalis</t>
-  </si>
-  <si>
-    <t>Ostoma septentrionalis Randall, 1838</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;septentrionalis&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Ostoma&lt;/em &lt;em&gt;septentrionalis&lt;/em&gt; Randall, 1838</t>
-  </si>
-  <si>
-    <t>Liriomyza equiseti De Meijere, 1924</t>
-  </si>
-  <si>
-    <t>Liriomyza equiseti</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Liriomyza&lt;/em&gt; &lt;em&gt;equiseti&lt;/em&gt; De Meijere, 1924</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Liriomyza&lt;/em&gt; &lt;em&gt;equiseti&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/1553334</t>
-  </si>
-  <si>
-    <t>Chirosia similata (Tiensuu, 1939)</t>
-  </si>
-  <si>
-    <t>Chirosia similata</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Chirosia&lt;/em&gt; &lt;em&gt;similata&lt;/em&gt; (Tiensuu, 1939)</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Chirosia&lt;/em&gt; &lt;em&gt;similata&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/1575323</t>
-  </si>
-  <si>
-    <t>Anthomyza gilviventris Roháček &amp; Barber, 2016</t>
-  </si>
-  <si>
-    <t>Anthomyza gilviventris</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Anthomyza&lt;/em&gt; &lt;em&gt;gilviventris&lt;/em&gt; Roháček &amp; Barber, 2016</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Anthomyza&lt;/em&gt; &lt;em&gt;gilviventris&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.researchgate.net/publication/312084641_Nearctic_Anthomyzidae_a_monograph_of_Anthomyza_and_allied_genera_Diptera</t>
-  </si>
-  <si>
-    <t>Lirula macrospora</t>
-  </si>
-  <si>
-    <t>Lirula macrospora (R.Hartig) Darker</t>
-  </si>
-  <si>
-    <t>Lirula needle blight</t>
-  </si>
-  <si>
-    <t>Lirula</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Lirula&lt;/em&gt; &lt;em&gt;macrospora&lt;/em&gt; (R.Hartig) Darker</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Lirula&lt;/em&gt; &lt;em&gt;macrospora&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/2579903</t>
-  </si>
-  <si>
-    <t>Lirula Darker</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/2579890</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Lirula&lt;/em&gt; Darker</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Lirula&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>Epipyxis gracilis</t>
-  </si>
-  <si>
-    <t>Epipyxis kenaiensis</t>
-  </si>
-  <si>
-    <t>Epipyxis planctonica</t>
-  </si>
-  <si>
-    <t>Epipyxis polymorpha</t>
-  </si>
-  <si>
-    <t>Synura petersenii</t>
-  </si>
-  <si>
-    <t>Synura petersenii Korshikov</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/3195206</t>
-  </si>
-  <si>
-    <t>Chromista|Species</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Synura&lt;/em&gt; &lt;em&gt;petersenii&lt;/em&gt; Korshikov</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Synura&lt;/em&gt; &lt;em&gt;petersenii&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>Epipyxis gracilis D.K.Hilliard &amp; Asmund</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/3195021</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;gracilis&lt;/em&gt; D.K.Hilliard &amp; Asmund</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;kenaiensis&lt;/em&gt; D.K.Hilliard &amp; Asmund</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;gracilis&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>Epipyxis kenaiensis D.K.Hilliard &amp; Asmund</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;kenaiensis&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/3195033</t>
-  </si>
-  <si>
-    <t>https://www.algaebase.org/search/species/detail/?species_id=112127</t>
-  </si>
-  <si>
-    <t>Epipyxis planctonica D.K.Hilliard &amp; B.C.Asmund</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;planctonica&lt;/em&gt; D.K.Hilliard &amp; B.C.Asmund</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;planctonica&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>Epipyxis polymorpha (J.W.G.Lund) D.K.Hilliard &amp; Asmund</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;polymorpha&lt;/em&gt; (J.W.G.Lund) D.K.Hilliard &amp; Asmund</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Epipyxis&lt;/em&gt; &lt;em&gt;polymorpha&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>https://www.gbif.org/species/3195019</t>
+    <t>Mycetophila evanida</t>
+  </si>
+  <si>
+    <t>Mycetophila evanida Lastovka, 1972</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Mycetophila&lt;/em&gt; &lt;em&gt;evanida&lt;/em&gt; Lastovka, 1972</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Mycetophila&lt;/em&gt; &lt;em&gt;evanida&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/1614155</t>
+  </si>
+  <si>
+    <t>Other Non-vertebrates|Species</t>
+  </si>
+  <si>
+    <t>Helobdella echoensis Saglam, Kutschera, Saunders, Saidel, Balombini &amp; Shain, 2018</t>
+  </si>
+  <si>
+    <t>Helobdella echoensis</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Helobdella&lt;/em&gt; &lt;em&gt;echoensis&lt;/em&gt; Saglam, Kutschera, Saunders, Saidel, Balombini &amp; Shain, 2018</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Helobdella&lt;/em&gt; &lt;em&gt;echoensis&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/9680041</t>
+  </si>
+  <si>
+    <t>Alnus alnobetula (Ehrh.) K.Koch</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Alnus&lt;/em&gt; &lt;em&gt;alnobetula&lt;/em&gt; (Ehrh.) K.Koch</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Alnus&lt;/em&gt; &lt;em&gt;alnobetula&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Alnus alnobetula</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/8956987|https://doi.org/10.3372/wi.41.41117|https://doi.org/10.3897/phytokeys.56.5225</t>
+  </si>
+  <si>
+    <t>Chrysomyxa ledicola Lagerh.</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Chrysomyxa&lt;/em&gt; &lt;em&gt;ledicola&lt;/em&gt; Lagerh.</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Chrysomyxa&lt;/em&gt; &lt;em&gt;ledicola&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Chrysomyxa ledicola</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/2513932</t>
+  </si>
+  <si>
+    <t>Chrysomyxa woroninii Tranzschel</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Chrysomyxa&lt;/em&gt; &lt;em&gt;woroninii&lt;/em&gt; Tranzschel</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Chrysomyxa&lt;/em&gt; &lt;em&gt;woroninii&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/2513947</t>
+  </si>
+  <si>
+    <t>Chrysomyxa woroninii</t>
+  </si>
+  <si>
+    <t>Cytospora notastroma Kepley &amp; F.B.Reeves, 2015</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Cytospora&lt;/em&gt; &lt;em&gt;notastroma&lt;/em&gt; Kepley &amp; F.B.Reeves, 2015</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Cytospora&lt;/em&gt; &lt;em&gt;notastroma&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Cytospora notastroma</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/9669747|https://www.mycobank.org/page/Name%20details%20page/name/Cytospora%20notastroma</t>
   </si>
 </sst>
 </file>
@@ -819,6 +711,16 @@
   <dxfs count="8">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -844,16 +746,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1401,11 +1293,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1469,7 +1361,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>116</v>
@@ -1484,7 +1376,7 @@
         <v>51</v>
       </c>
       <c r="G2" s="12">
-        <v>627969</v>
+        <v>26160</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>120</v>
@@ -1498,80 +1390,80 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>123</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>122</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G3" s="12">
-        <v>555212</v>
+        <v>563836</v>
       </c>
       <c r="K3" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="L3" s="12" t="s">
-        <v>124</v>
-      </c>
       <c r="M3" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>128</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>129</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="12">
-        <v>555212</v>
+        <v>101988</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>130</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>133</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>132</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G5" s="12">
-        <v>49281</v>
+        <v>1006245</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>135</v>
@@ -1580,27 +1472,27 @@
         <v>134</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G6" s="12">
-        <v>56467</v>
+        <v>1006245</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>140</v>
@@ -1614,22 +1506,22 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="12">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>143</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>142</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G7" s="12">
-        <v>42303</v>
+        <v>100166</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>145</v>
@@ -1638,230 +1530,28 @@
         <v>144</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="12">
-        <v>7</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="12" t="s">
         <v>147</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="12">
-        <v>8</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="12">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="12">
-        <v>388655</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="12">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="12">
-        <v>63440</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="12">
-        <v>10</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="12">
-        <v>63440</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="12">
-        <v>63440</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="12">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="12">
-        <v>63440</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="12">
-        <v>13</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="12">
-        <v>68346</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C6 C8:C1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="11"/>
+  <conditionalFormatting sqref="C1:C5 C7:C1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sci. Name w/auth. text" error="Scientific Name with Authority must be text between 3 and 175 characters in length." sqref="D1:D1048576 C7">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Scientific Name text" error="Scientific Name must be text between 2 and 87 characters in length." sqref="C1:C5 C7:C1048576">
+      <formula1>2</formula1>
+      <formula2>87</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sci. Name w/auth. text" error="Scientific Name with Authority must be text between 3 and 175 characters in length." sqref="D1:D1048576 C6">
       <formula1>3</formula1>
       <formula2>175</formula2>
     </dataValidation>
@@ -1869,15 +1559,11 @@
       <formula1>1</formula1>
       <formula2>63000</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Scientific Name text" error="Scientific Name must be text between 2 and 87 characters in length." sqref="C1:C6 C8:C1048576">
-      <formula1>2</formula1>
-      <formula2>87</formula2>
-    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
-      <formula1>$A$2:$A$923</formula1>
+      <formula1>$A$2:$A$910</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2205,16 +1891,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A6:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6 C1 C8:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D1 D9:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="5">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1 G6 G8:G1048576">
@@ -5838,44 +5524,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5921,16 +5569,45 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6148,7 +5825,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
@@ -6165,23 +5859,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6198,4 +5876,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>